<commit_message>
Added the Widgets Page And TestCases
</commit_message>
<xml_diff>
--- a/in.automationtest/src/test/resources/MasterTestData.xlsx
+++ b/in.automationtest/src/test/resources/MasterTestData.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efrain\Java_practice_workspace\com.letskodeit.teachable\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efrain\git\in.automationtest\in.automationtest\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F8095C-EC21-451F-A650-76E4E1593267}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16230" windowHeight="9030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="com.letskodeit.teachable" sheetId="1" r:id="rId1"/>
+    <sheet name="in.automationtest" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'com.letskodeit.teachable'!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">in.automationtest!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,42 +28,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
-    <t>BMW</t>
+    <t>countries</t>
   </si>
   <si>
-    <t>Benz</t>
+    <t>United States,Panama,Zimbabwe</t>
   </si>
   <si>
-    <t>Honda</t>
+    <t>countryNames</t>
   </si>
   <si>
-    <t>auto</t>
-  </si>
-  <si>
-    <t>SelectPractice</t>
-  </si>
-  <si>
-    <t>Apple Orange Peach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peach Orange </t>
-  </si>
-  <si>
-    <t>Orange</t>
-  </si>
-  <si>
-    <t>MultipleAutos</t>
-  </si>
-  <si>
-    <t>MultipleColors</t>
-  </si>
-  <si>
-    <t>BMW Benz Honda</t>
-  </si>
-  <si>
-    <t>Honda Benz</t>
+    <t>New Zealand,Argentina,Puerto Rico</t>
   </si>
 </sst>
 </file>
@@ -98,9 +75,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,107 +391,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="2" max="2" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:B1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added data for registration data provider
</commit_message>
<xml_diff>
--- a/in.automationtest/src/test/resources/MasterTestData.xlsx
+++ b/in.automationtest/src/test/resources/MasterTestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efrain\git\in.automationtest\in.automationtest\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F8095C-EC21-451F-A650-76E4E1593267}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8EA6D9-9DEA-45E4-A3EF-BEEC0ED1B5A0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16230" windowHeight="9030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>countries</t>
   </si>
@@ -40,6 +40,33 @@
   </si>
   <si>
     <t>New Zealand,Argentina,Puerto Rico</t>
+  </si>
+  <si>
+    <t>registration</t>
+  </si>
+  <si>
+    <t>eis_cpa@yahoo.com</t>
+  </si>
+  <si>
+    <t>Elena</t>
+  </si>
+  <si>
+    <t>44 Brandywine cir</t>
+  </si>
+  <si>
+    <t>spanish</t>
+  </si>
+  <si>
+    <t>Programming</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>United States of America</t>
+  </si>
+  <si>
+    <t>Elenaau12</t>
   </si>
 </sst>
 </file>
@@ -391,19 +418,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" customWidth="1"/>
+    <col min="12" max="12" width="5" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -411,7 +447,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -419,7 +455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -427,12 +463,53 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>7324242995</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5">
+        <v>1968</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>21</v>
+      </c>
+      <c r="M5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test date for recordVerification Data Provider
</commit_message>
<xml_diff>
--- a/in.automationtest/src/test/resources/MasterTestData.xlsx
+++ b/in.automationtest/src/test/resources/MasterTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efrain\git\in.automationtest\in.automationtest\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8EA6D9-9DEA-45E4-A3EF-BEEC0ED1B5A0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82CDB56-60E4-45E8-B167-76500035D1C1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16230" windowHeight="9030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>countries</t>
   </si>
@@ -67,16 +67,33 @@
   </si>
   <si>
     <t>Elenaau12</t>
+  </si>
+  <si>
+    <t>recordVerification</t>
+  </si>
+  <si>
+    <t>111@gmail.com</t>
+  </si>
+  <si>
+    <t>beto@bob.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,13 +116,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -418,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,9 +532,29 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{0D6251F4-A4B8-42DA-B19A-C51CB9A524DC}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{7FD12B00-903C-4AC7-9CC4-53AFF0EE1735}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>